<commit_message>
ui finished and all processes running off npm run start
</commit_message>
<xml_diff>
--- a/api/milestones.xlsx
+++ b/api/milestones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3dtholdings-my.sharepoint.com/personal/bpatel_calmi2_org/Documents/Bhavesh/SPARC/SODA - Phase 3/New hire/Frontend post/Interview exercise/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacobi\programming\projects\Milestones\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4F9D37E-4612-4974-A545-8DAFE16A34E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92EDA2E-0763-446F-8D35-7586FC9DD7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="1320" windowWidth="23760" windowHeight="13635" xr2:uid="{9176C2F8-AFF7-4368-876B-F4F4FBD1E566}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{9176C2F8-AFF7-4368-876B-F4F4FBD1E566}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,16 +438,16 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -455,7 +455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -463,7 +463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -471,7 +471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -479,7 +479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -487,7 +487,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -495,7 +495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>

</xml_diff>